<commit_message>
2014 03 24 18:19
ciração a agenta de progeto
</commit_message>
<xml_diff>
--- a/BD2_2M/T2 - Funções/Agenda de projeto.xlsx
+++ b/BD2_2M/T2 - Funções/Agenda de projeto.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$21</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="37">
   <si>
     <t>Ação</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Aurélio</t>
   </si>
   <si>
-    <t xml:space="preserve">Estrurura da atividade </t>
-  </si>
-  <si>
     <t>GitHub</t>
   </si>
   <si>
@@ -110,13 +107,52 @@
     <t>!</t>
   </si>
   <si>
-    <t>Atividades estão detalhadas no arquivo "02 Exercício de View em PostgreSQL ALUNO x DISCIPLINA.pdf"</t>
-  </si>
-  <si>
     <t>Ativid:</t>
   </si>
   <si>
     <t>Pasta T1 - Funções</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estrutura da atividade </t>
+  </si>
+  <si>
+    <t>Tabela tipoUtilitario</t>
+  </si>
+  <si>
+    <t>notpad++</t>
+  </si>
+  <si>
+    <t>Tabela Utilitarios</t>
+  </si>
+  <si>
+    <t>||</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t>Tabela Material</t>
+  </si>
+  <si>
+    <t>Tabela ItensNf</t>
+  </si>
+  <si>
+    <t>Tabela NotaFiscal</t>
+  </si>
+  <si>
+    <t>Função 1</t>
+  </si>
+  <si>
+    <t>Função 2</t>
+  </si>
+  <si>
+    <t>Função 3</t>
+  </si>
+  <si>
+    <t>Atividades estão detalhadas no arquivo "BD2 Trabalho Funçoes NF OK.pdff"</t>
+  </si>
+  <si>
+    <t>Obs todas as tabélas e funções serão em aquivos individuais</t>
   </si>
 </sst>
 </file>
@@ -150,20 +186,19 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="23">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,12 +286,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFABF8F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -322,46 +351,37 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -374,21 +394,30 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,7 +445,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -459,7 +488,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -780,82 +809,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="57" style="22" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="24" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="21" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="21" customWidth="1"/>
-    <col min="7" max="7" width="23" style="22" customWidth="1"/>
-    <col min="8" max="8" width="53" style="22" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="57" style="19" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="21" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="18" customWidth="1"/>
+    <col min="7" max="7" width="23" style="21" customWidth="1"/>
+    <col min="8" max="8" width="30" style="19" customWidth="1"/>
     <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="20" customFormat="1" ht="15">
-      <c r="A1" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+    <row r="1" spans="1:8" s="17" customFormat="1" ht="15">
+      <c r="A1" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="7"/>
-      <c r="G1" s="8"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" ht="14.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
+    <row r="2" spans="1:8" ht="21" customHeight="1">
+      <c r="A2" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" ht="33.75" customHeight="1">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="24" customHeight="1">
+    <row r="4" spans="1:8" ht="21" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -867,19 +898,19 @@
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="24" customHeight="1">
+    <row r="5" spans="1:8" ht="21" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -888,184 +919,391 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="24" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
+    <row r="6" spans="1:8" ht="21" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="24" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="24" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
+    <row r="7" spans="1:8" ht="21" customHeight="1">
+      <c r="A7" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="18">
+        <v>3</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="21" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="24" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
+    <row r="9" spans="1:8" ht="21" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="24" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="24" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
+    <row r="10" spans="1:8" ht="21" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="24" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="24" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="24" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="25.5" customHeight="1">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
+    <row r="12" spans="1:8" ht="21" customHeight="1">
+      <c r="A12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="18">
+        <v>5</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1">
+      <c r="A13" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="18">
+        <v>5</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="3">
+        <v>6</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="24" customHeight="1">
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="24" customHeight="1">
+    <row r="16" spans="1:8" ht="21" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="21" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D17" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" ht="21" customHeight="1">
+      <c r="A18" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="18">
+        <v>10</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" ht="21" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="3">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="21" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="3">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" s="20" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="B21" s="22">
+        <f>COUNTA(B4:B20)</f>
         <v>17</v>
       </c>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="24" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="3">
-        <v>11</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" s="23" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="25">
-        <f>COUNTA(B4:B18)</f>
-        <v>4</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G19">
+  <autoFilter ref="A3:G21">
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
   </autoFilter>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:D2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
2014 03 22 12:55
tabelas e funções somente aguardando testes para serem envidas
</commit_message>
<xml_diff>
--- a/BD2_2M/T2 - Funções/Agenda de projeto.xlsx
+++ b/BD2_2M/T2 - Funções/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$21</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1098,7 +1098,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>24</v>
@@ -1121,7 +1121,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>24</v>
@@ -1144,7 +1144,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>24</v>
@@ -1167,7 +1167,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>24</v>
@@ -1191,7 +1191,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>24</v>
@@ -1215,7 +1215,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>24</v>
@@ -1239,7 +1239,7 @@
         <v>9</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G18" s="21" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
2014 03 31 12:54
Testes nas tabel
</commit_message>
<xml_diff>
--- a/BD2_2M/T2 - Funções/Agenda de projeto.xlsx
+++ b/BD2_2M/T2 - Funções/Agenda de projeto.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\BD\BD2_2M\T2 - Funções\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$21</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -22,7 +27,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -80,9 +85,6 @@
     <t>Neimar</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Aurélio</t>
   </si>
   <si>
@@ -159,13 +161,16 @@
   </si>
   <si>
     <t xml:space="preserve">Todas as tabelas e funções </t>
+  </si>
+  <si>
+    <t>?!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -351,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -419,9 +424,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -441,6 +443,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -534,6 +539,49 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 23" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -580,7 +628,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -612,9 +660,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -646,6 +695,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -821,14 +871,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="19" customWidth="1"/>
     <col min="2" max="2" width="57" style="19" customWidth="1"/>
@@ -841,31 +891,31 @@
     <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="17" customFormat="1" ht="15">
-      <c r="A1" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+    <row r="1" spans="1:8" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="7"/>
       <c r="G1" s="23"/>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1">
-      <c r="A2" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="8"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:8" ht="33.75" customHeight="1">
+    <row r="3" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -891,15 +941,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21" customHeight="1">
+    <row r="4" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -908,22 +958,22 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1">
+    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -932,22 +982,22 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1">
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -956,22 +1006,22 @@
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1">
+    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="18">
         <v>3</v>
@@ -979,22 +1029,22 @@
       <c r="E7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="24" t="s">
-        <v>19</v>
+      <c r="F7" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="21" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="3">
         <v>3</v>
@@ -1003,22 +1053,22 @@
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="D9" s="3">
         <v>3</v>
@@ -1027,22 +1077,22 @@
         <v>9</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1">
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3">
         <v>4</v>
@@ -1051,21 +1101,21 @@
         <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="3">
         <v>4</v>
@@ -1074,45 +1124,45 @@
         <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1">
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="18">
         <v>5</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="18">
         <v>5</v>
@@ -1120,45 +1170,45 @@
       <c r="E13" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>19</v>
+      <c r="F13" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="21" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="3">
         <v>6</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="21" customHeight="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="3">
         <v>6</v>
@@ -1167,22 +1217,22 @@
         <v>9</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="21" customHeight="1">
+    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="3">
         <v>7</v>
@@ -1191,46 +1241,46 @@
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="21" customHeight="1">
+    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="3">
         <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="21" customHeight="1">
+    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="18">
         <v>10</v>
@@ -1239,46 +1289,46 @@
         <v>9</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" ht="21" customHeight="1">
+    <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="3">
         <v>11</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" ht="21" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D20" s="3">
         <v>12</v>
@@ -1287,16 +1337,16 @@
         <v>9</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" s="20" customFormat="1" ht="26.25" customHeight="1">
+    <row r="21" spans="1:8" s="20" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="22">
         <f>COUNTA(B4:B20)</f>
@@ -1310,10 +1360,7 @@
       <c r="H21" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G21">
-    <filterColumn colId="4"/>
-    <filterColumn colId="5"/>
-  </autoFilter>
+  <autoFilter ref="A3:G21"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>